<commit_message>
upd invoice_generator.py, invoice_sheet_functions.py, test file, xlsx data
</commit_message>
<xml_diff>
--- a/src/python/comp-230/test_invoice_data.xlsx
+++ b/src/python/comp-230/test_invoice_data.xlsx
@@ -7,17 +7,17 @@
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12240" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Test_Customers" sheetId="1" r:id="rId1"/>
-    <sheet name="Test_Invoices" sheetId="2" r:id="rId2"/>
-    <sheet name="Test_Products" sheetId="3" r:id="rId3"/>
-    <sheet name="Test_Line Items" sheetId="4" r:id="rId4"/>
+    <sheet name="Customers" sheetId="1" r:id="rId1"/>
+    <sheet name="Invoices" sheetId="2" r:id="rId2"/>
+    <sheet name="Products" sheetId="3" r:id="rId3"/>
+    <sheet name="Line Items" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>PROD_ID</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>test2@test2.com</t>
+  </si>
+  <si>
+    <t>LINE_ID</t>
   </si>
 </sst>
 </file>
@@ -513,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,77 +788,92 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>101</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>101</v>
       </c>
       <c r="C2" s="5">
+        <v>101</v>
+      </c>
+      <c r="D2" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>102</v>
+      </c>
+      <c r="B3" s="5">
         <v>101</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="5">
         <v>102</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D3" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>103</v>
+      </c>
+      <c r="B4" s="5">
         <v>102</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="5">
         <v>101</v>
       </c>
-      <c r="C4" s="5">
+      <c r="D4" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>104</v>
+      </c>
+      <c r="B5" s="5">
         <v>102</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="5">
         <v>102</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="5">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>